<commit_message>
XONG ROI NHUNG SUA THEM 1 SỐ cái
</commit_message>
<xml_diff>
--- a/MVCExample/nhanvien.xlsx
+++ b/MVCExample/nhanvien.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t>Quản lý nhân viên</t>
   </si>
@@ -44,55 +44,55 @@
     <t>Hoang Huy</t>
   </si>
   <si>
-    <t>1132546</t>
+    <t>0376169671</t>
   </si>
   <si>
     <t>HN</t>
   </si>
   <si>
-    <t>Nhan vien</t>
+    <t>Nhan Vien</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>NV-0002</t>
+  </si>
+  <si>
+    <t>Duong A</t>
+  </si>
+  <si>
+    <t>03468</t>
+  </si>
+  <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>NV-0003</t>
+  </si>
+  <si>
+    <t>Van B</t>
+  </si>
+  <si>
+    <t>061516</t>
+  </si>
+  <si>
+    <t>Truong phong</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>NV-0002</t>
-  </si>
-  <si>
-    <t>Duong Van</t>
-  </si>
-  <si>
-    <t>031546</t>
-  </si>
-  <si>
-    <t>LS</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>NV-0003</t>
-  </si>
-  <si>
-    <t>Hoang</t>
-  </si>
-  <si>
-    <t>013</t>
-  </si>
-  <si>
-    <t>Truong Phong</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>NV-0004</t>
   </si>
   <si>
-    <t>Van A</t>
-  </si>
-  <si>
-    <t>012313</t>
+    <t xml:space="preserve">Hoang </t>
+  </si>
+  <si>
+    <t>013156</t>
   </si>
   <si>
     <t>Giam Doc</t>
@@ -101,97 +101,256 @@
     <t>NV-0005</t>
   </si>
   <si>
+    <t>Hung</t>
+  </si>
+  <si>
+    <t>013161</t>
+  </si>
+  <si>
+    <t>Ke toan</t>
+  </si>
+  <si>
+    <t>NV-0006</t>
+  </si>
+  <si>
+    <t>Van Thanh</t>
+  </si>
+  <si>
+    <t>01616</t>
+  </si>
+  <si>
+    <t>Thu Ky</t>
+  </si>
+  <si>
+    <t>NV-0007</t>
+  </si>
+  <si>
+    <t>Van C</t>
+  </si>
+  <si>
+    <t>016333</t>
+  </si>
+  <si>
+    <t>NV-0008</t>
+  </si>
+  <si>
+    <t>Hoang Phong</t>
+  </si>
+  <si>
+    <t>0132456</t>
+  </si>
+  <si>
+    <t>NV-0009</t>
+  </si>
+  <si>
     <t>Duong B</t>
   </si>
   <si>
-    <t>0134156</t>
+    <t>0132546</t>
+  </si>
+  <si>
+    <t>NV-0011</t>
+  </si>
+  <si>
+    <t>Duong Cong</t>
+  </si>
+  <si>
+    <t>01498</t>
+  </si>
+  <si>
+    <t>NV-0012</t>
+  </si>
+  <si>
+    <t>Dung Van</t>
+  </si>
+  <si>
+    <t>0123456</t>
+  </si>
+  <si>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>NV-0013</t>
+  </si>
+  <si>
+    <t>0132</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>NV-0014</t>
+  </si>
+  <si>
+    <t>Than</t>
+  </si>
+  <si>
+    <t>NV-0015</t>
+  </si>
+  <si>
+    <t>Hong</t>
+  </si>
+  <si>
+    <t>0136</t>
+  </si>
+  <si>
+    <t>Thu ky</t>
+  </si>
+  <si>
+    <t>NV-0016</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>NV-0017</t>
+  </si>
+  <si>
+    <t>Ba</t>
+  </si>
+  <si>
+    <t>16161616</t>
+  </si>
+  <si>
+    <t>NV-0018</t>
+  </si>
+  <si>
+    <t>Duong Van Tu</t>
+  </si>
+  <si>
+    <t>NV-0019</t>
+  </si>
+  <si>
+    <t>Hoang 19</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>NV-0020</t>
+  </si>
+  <si>
+    <t>Hoang20@gmail.com</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>NV-0021</t>
+  </si>
+  <si>
+    <t>Duong Duong</t>
+  </si>
+  <si>
+    <t>NV-0022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huy Hoang </t>
+  </si>
+  <si>
+    <t>0789</t>
   </si>
   <si>
     <t>BN</t>
   </si>
   <si>
-    <t>NV-0006</t>
-  </si>
-  <si>
-    <t>Nguyen</t>
-  </si>
-  <si>
-    <t>0132456</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>NV-0007</t>
-  </si>
-  <si>
-    <t>Ba</t>
-  </si>
-  <si>
-    <t>NV-0008</t>
-  </si>
-  <si>
-    <t>Nguyen Van A</t>
-  </si>
-  <si>
-    <t>0123546</t>
-  </si>
-  <si>
-    <t>Thu ky</t>
-  </si>
-  <si>
-    <t>NV-0009</t>
-  </si>
-  <si>
-    <t>Duong Nguyen</t>
-  </si>
-  <si>
-    <t>0489</t>
-  </si>
-  <si>
-    <t>NV-0010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anh </t>
-  </si>
-  <si>
-    <t>0436</t>
-  </si>
-  <si>
-    <t>NV-0011</t>
-  </si>
-  <si>
-    <t>013465</t>
-  </si>
-  <si>
-    <t>NV-0012</t>
-  </si>
-  <si>
-    <t>Huy Duong</t>
-  </si>
-  <si>
-    <t>0376169123</t>
-  </si>
-  <si>
-    <t>NV-0013</t>
-  </si>
-  <si>
-    <t>hoang abc @mgial.com</t>
-  </si>
-  <si>
-    <t>0346</t>
-  </si>
-  <si>
-    <t>NV-0015</t>
-  </si>
-  <si>
-    <t>huy@gmailc</t>
+    <t>NV-0023</t>
+  </si>
+  <si>
+    <t>Huy23</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>NV-0024</t>
+  </si>
+  <si>
+    <t>huy245</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>3123</t>
+  </si>
+  <si>
+    <t>NV-0025</t>
+  </si>
+  <si>
+    <t>huy25</t>
   </si>
   <si>
     <t>123</t>
   </si>
   <si>
-    <t>132</t>
+    <t>NV-0026</t>
+  </si>
+  <si>
+    <t>huy26</t>
+  </si>
+  <si>
+    <t>NV-0027</t>
+  </si>
+  <si>
+    <t>huy27</t>
+  </si>
+  <si>
+    <t>213</t>
+  </si>
+  <si>
+    <t>NV-0028</t>
+  </si>
+  <si>
+    <t>1241</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>NV-0029</t>
+  </si>
+  <si>
+    <t>124124</t>
+  </si>
+  <si>
+    <t>214</t>
+  </si>
+  <si>
+    <t>NV-0030</t>
+  </si>
+  <si>
+    <t>123213</t>
+  </si>
+  <si>
+    <t>NV-0031</t>
+  </si>
+  <si>
+    <t>24124</t>
+  </si>
+  <si>
+    <t>NV-0032</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>NV-0033</t>
+  </si>
+  <si>
+    <t>33@@</t>
+  </si>
+  <si>
+    <t>NV-0034</t>
+  </si>
+  <si>
+    <t>312</t>
+  </si>
+  <si>
+    <t>NV-0035</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -387,7 +546,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -493,7 +652,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="4">
-        <v>35866</v>
+        <v>36421</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>16</v>
@@ -516,13 +675,13 @@
         <v>20</v>
       </c>
       <c r="C6" s="4">
-        <v>36628</v>
+        <v>36157</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>22</v>
@@ -539,19 +698,19 @@
         <v>25</v>
       </c>
       <c r="C7" s="4">
-        <v>42084</v>
+        <v>36046</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>27</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
@@ -562,19 +721,19 @@
         <v>29</v>
       </c>
       <c r="C8" s="4">
-        <v>35866</v>
+        <v>30818</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="G8" s="16" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
@@ -585,19 +744,19 @@
         <v>33</v>
       </c>
       <c r="C9" s="4">
-        <v>36534</v>
+        <v>42265</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>35</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
@@ -608,42 +767,42 @@
         <v>37</v>
       </c>
       <c r="C10" s="4">
-        <v>35041</v>
+        <v>41251</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" s="4">
-        <v>36262</v>
+        <v>31537</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12">
@@ -654,19 +813,19 @@
         <v>43</v>
       </c>
       <c r="C12" s="4">
-        <v>35897</v>
+        <v>36647</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
@@ -677,16 +836,16 @@
         <v>46</v>
       </c>
       <c r="C13" s="4">
-        <v>36011</v>
+        <v>-15</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>23</v>
@@ -697,59 +856,59 @@
         <v>48</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C14" s="4">
-        <v>21781</v>
+        <v>35201</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="C15" s="4">
-        <v>36534</v>
+        <v>35773</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="4">
+        <v>35528</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="4">
-        <v>36544</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>17</v>
@@ -762,26 +921,486 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="7">
-        <v>36879</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="B17" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="6" t="s">
+      <c r="C17" s="4">
+        <v>36142</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="E17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="16" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="4">
+        <v>36512</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="4">
+        <v>-4035</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="4">
+        <v>32126</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="4">
+        <v>36513</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="4">
+        <v>36513</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="4">
+        <v>36147</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="4">
+        <v>32739</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="4">
+        <v>36513</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="4">
+        <v>-648871</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="4">
+        <v>-616092</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="4">
+        <v>-648964</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="4">
+        <v>-648567</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="4">
+        <v>-648567</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="4">
+        <v>-609509</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" s="4">
+        <v>-648567</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" s="4">
+        <v>-543408</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" s="4">
+        <v>-648964</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="4">
+        <v>-648964</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="7">
+        <v>-648964</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>